<commit_message>
Update sheet query range
</commit_message>
<xml_diff>
--- a/source.xlsx
+++ b/source.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Mr.</t>
   </si>
@@ -84,6 +84,18 @@
   </si>
   <si>
     <t>Ordinary Guy</t>
+  </si>
+  <si>
+    <t>xTestWordx</t>
+  </si>
+  <si>
+    <t>Wassap</t>
+  </si>
+  <si>
+    <t>Hahahaha</t>
+  </si>
+  <si>
+    <t>Yowz</t>
   </si>
 </sst>
 </file>
@@ -402,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,7 +428,7 @@
     <col min="4" max="4" width="39.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -432,8 +444,11 @@
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -449,8 +464,11 @@
       <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -466,8 +484,11 @@
       <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -482,6 +503,9 @@
       </c>
       <c r="E4" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved to specify source and template files
Script now allows user to specify the source and template files. The readme.md is also update to reflect these features.
</commit_message>
<xml_diff>
--- a/source.xlsx
+++ b/source.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
   <si>
     <t>Mr.</t>
   </si>
@@ -96,6 +96,18 @@
   </si>
   <si>
     <t>Yowz</t>
+  </si>
+  <si>
+    <t>xTestWord2x</t>
+  </si>
+  <si>
+    <t>Test Doc 4</t>
+  </si>
+  <si>
+    <t>Test Doc 5</t>
+  </si>
+  <si>
+    <t>Test Doc 6</t>
   </si>
 </sst>
 </file>
@@ -414,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,9 +438,10 @@
     <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="3" width="26.140625" customWidth="1"/>
     <col min="4" max="4" width="39.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -447,8 +460,11 @@
       <c r="F1" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -467,8 +483,11 @@
       <c r="F2" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -487,8 +506,11 @@
       <c r="F3" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -506,6 +528,78 @@
       </c>
       <c r="F4" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>